<commit_message>
First major commit (Python)
</commit_message>
<xml_diff>
--- a/MS2000 Export.xlsx
+++ b/MS2000 Export.xlsx
@@ -596,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EA184"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="BV169" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="CK184" sqref="CK184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>